<commit_message>
Actualiza excel de medidas
</commit_message>
<xml_diff>
--- a/Pruebas apertura horizontal.xlsx
+++ b/Pruebas apertura horizontal.xlsx
@@ -287,11 +287,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="737763040"/>
-        <c:axId val="737102144"/>
+        <c:axId val="896678768"/>
+        <c:axId val="896681520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="737763040"/>
+        <c:axId val="896678768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,7 +348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="737102144"/>
+        <c:crossAx val="896681520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -356,7 +356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="737102144"/>
+        <c:axId val="896681520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,7 +412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="737763040"/>
+        <c:crossAx val="896678768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1315,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1480,6 +1480,12 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
     </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D16">
+        <f>MAX(D2:D10)</f>
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>